<commit_message>
Feat #9420 ter (#9448)
* create group on source upload + improve

* cleaning

* WIP import groups

* debug

* cleaning

* improvment: can put title instead of id

* allow more lines for documents import

* small debug

* typo

* small improvments & debug

---------

Co-authored-by: bruce <delorme.bruce.michel@gmail.com>
</commit_message>
<xml_diff>
--- a/assets/templates/import-sources-template.xlsx
+++ b/assets/templates/import-sources-template.xlsx
@@ -93,7 +93,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Destination ID
+      <t xml:space="preserve">Destination Ids
 </t>
     </r>
     <r>
@@ -105,7 +105,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">// The rightId this income will go to</t>
+      <t xml:space="preserve">// The rightIds this income will go to</t>
     </r>
   </si>
 </sst>
@@ -340,16 +340,16 @@
   <dimension ref="A10:Y40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.35"/>
   </cols>
   <sheetData>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Feat 9420 5 state reader (#9461)
* debug & improved graph-component

* cleaned sources

* casablancas fixes

* updated source templte

* improvments & debug

* chanded incomes order

* new actiobs, debugs, order column for vertical groups

* debug & new condition

* wip state reader

* vertical groups into horizontal

* cleaning debug & improvments

---------

Co-authored-by: bruce <delorme.bruce.michel@gmail.com>
</commit_message>
<xml_diff>
--- a/assets/templates/import-sources-template.xlsx
+++ b/assets/templates/import-sources-template.xlsx
@@ -93,7 +93,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Destination Ids
+      <t xml:space="preserve">Destination Id
 </t>
     </r>
     <r>
@@ -105,7 +105,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">// The rightIds this income will go to</t>
+      <t xml:space="preserve">// The rightId this income will go to</t>
     </r>
   </si>
 </sst>
@@ -239,7 +239,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,7 +256,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,16 +344,17 @@
   <dimension ref="A10:Y40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10:G10"/>
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.76"/>
   </cols>
   <sheetData>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -395,273 +400,273 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>